<commit_message>
tested different svm kernerls and generated report
</commit_message>
<xml_diff>
--- a/classifiers/github_labels/svm/report.xlsx
+++ b/classifiers/github_labels/svm/report.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t>Kernel</t>
   </si>
@@ -46,13 +47,37 @@
   </si>
   <si>
     <t>linear</t>
+  </si>
+  <si>
+    <t>rbf</t>
+  </si>
+  <si>
+    <t>99 by 100</t>
+  </si>
+  <si>
+    <t>95 by 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rbf </t>
+  </si>
+  <si>
+    <t>95 by 100</t>
+  </si>
+  <si>
+    <t>95 by 10</t>
+  </si>
+  <si>
+    <t>90 by 5</t>
+  </si>
+  <si>
+    <t>poly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,8 +100,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,6 +125,22 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -113,15 +168,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
@@ -435,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +543,285 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>65.25</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>72.010000000000005</v>
+      </c>
+      <c r="G3">
+        <v>6.07</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>74.69</v>
+      </c>
+      <c r="G4">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>73.63</v>
+      </c>
+      <c r="G5">
+        <v>6.4</v>
+      </c>
+      <c r="H5">
+        <v>6.1870000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>65.430000000000007</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>65.430000000000007</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>67.010000000000005</v>
+      </c>
+      <c r="G8">
+        <v>6.6</v>
+      </c>
+      <c r="H8">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2">
+        <v>75.92</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5.9</v>
+      </c>
+      <c r="H9" s="2">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>100000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>72.39</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1000000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2">
+        <v>76.84</v>
+      </c>
+      <c r="G12" s="2">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="H12" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="4">
+        <v>80.08</v>
+      </c>
+      <c r="G13" s="3">
+        <v>432</v>
+      </c>
+      <c r="H13" s="3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated some old classifiers and their reports
Added:
k nearest neighbour classfier + report
Updated report for: SVM
</commit_message>
<xml_diff>
--- a/classifiers/github_labels/svm/report.xlsx
+++ b/classifiers/github_labels/svm/report.xlsx
@@ -500,7 +500,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,9 +787,15 @@
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="2">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1394</v>
+      </c>
+      <c r="H14" s="3">
+        <v>490</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -799,7 +805,16 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>65</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -810,10 +825,19 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>65.430000000000007</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -821,7 +845,16 @@
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>65.430000000000007</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>